<commit_message>
Add gunicorn and setup for Render
</commit_message>
<xml_diff>
--- a/donnees.xlsx
+++ b/donnees.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,20 @@
       </c>
       <c r="D7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>mskdgjmsldfgmdsfgjdsmfg</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2342354</v>
+      </c>
+      <c r="C8" t="n">
+        <v>324252346.5</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>